<commit_message>
Revert "Revert "Docs: 更新excel檔""
</commit_message>
<xml_diff>
--- a/data_excel/109.xlsx
+++ b/data_excel/109.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>1</t>
   </si>
@@ -138,6 +138,16 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被</t>
+  </si>
+  <si>
+    <t>passive</t>
+  </si>
+  <si>
+    <t>虛詞</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -145,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +177,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -199,13 +217,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -508,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -556,7 +614,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -576,15 +634,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -598,13 +656,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -618,13 +676,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -635,72 +693,83 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>